<commit_message>
Add a sheet dropdown which updates with the names of the sheets
</commit_message>
<xml_diff>
--- a/ExcelImport/ExampleSage50Export.xlsx
+++ b/ExcelImport/ExampleSage50Export.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="10215" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sage 50 journals export" sheetId="1" r:id="rId1"/>
+    <sheet name="Unrelated data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19764" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19768" uniqueCount="680">
   <si>
     <t>No</t>
   </si>
@@ -2056,6 +2057,15 @@
   <si>
     <t>78</t>
   </si>
+  <si>
+    <t>Divisional output</t>
+  </si>
+  <si>
+    <t>Widgets bought</t>
+  </si>
+  <si>
+    <t>Widgets sold</t>
+  </si>
 </sst>
 </file>
 
@@ -2064,7 +2074,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="?"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2075,6 +2085,35 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2118,10 +2157,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2133,8 +2173,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2415,7 +2489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1236"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -79039,4 +79113,787 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D100"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="14"/>
+    <col min="3" max="3" width="9.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>678</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>677</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>41839</v>
+      </c>
+      <c r="B2" s="11">
+        <v>5</v>
+      </c>
+      <c r="C2" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D2" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>41842</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12">
+        <v>3316</v>
+      </c>
+      <c r="D3" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>41843</v>
+      </c>
+      <c r="B4" s="11">
+        <v>3</v>
+      </c>
+      <c r="C4" s="12">
+        <v>5617</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>41849</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12">
+        <v>1500</v>
+      </c>
+      <c r="D5" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>41850</v>
+      </c>
+      <c r="B6" s="11">
+        <v>0</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1500</v>
+      </c>
+      <c r="D6" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>41853</v>
+      </c>
+      <c r="B7" s="11">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>41858</v>
+      </c>
+      <c r="B8" s="11">
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>41860</v>
+      </c>
+      <c r="B9" s="11">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>41867</v>
+      </c>
+      <c r="B10" s="11">
+        <v>2</v>
+      </c>
+      <c r="C10" s="12">
+        <v>25468</v>
+      </c>
+      <c r="D10" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>41875</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12">
+        <v>43217</v>
+      </c>
+      <c r="D11" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>41878</v>
+      </c>
+      <c r="B12" s="11">
+        <v>3</v>
+      </c>
+      <c r="C12" s="12">
+        <v>11245</v>
+      </c>
+      <c r="D12" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>41881</v>
+      </c>
+      <c r="B13" s="11">
+        <v>0</v>
+      </c>
+      <c r="C13" s="12">
+        <v>17930</v>
+      </c>
+      <c r="D13" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>41895</v>
+      </c>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="C14" s="12">
+        <v>40799</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>41902</v>
+      </c>
+      <c r="B15" s="11">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <v>20026</v>
+      </c>
+      <c r="D15" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>41905</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12">
+        <v>17353</v>
+      </c>
+      <c r="D16" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>41909</v>
+      </c>
+      <c r="B17" s="11">
+        <v>0</v>
+      </c>
+      <c r="C17" s="12">
+        <v>41325</v>
+      </c>
+      <c r="D17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>41916</v>
+      </c>
+      <c r="B18" s="11">
+        <v>3</v>
+      </c>
+      <c r="C18" s="12">
+        <v>42713</v>
+      </c>
+      <c r="D18" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>41930</v>
+      </c>
+      <c r="B19" s="11">
+        <v>0</v>
+      </c>
+      <c r="C19" s="12">
+        <v>29615</v>
+      </c>
+      <c r="D19" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>41937</v>
+      </c>
+      <c r="B20" s="11">
+        <v>0</v>
+      </c>
+      <c r="C20" s="12">
+        <v>44449</v>
+      </c>
+      <c r="D20" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>41946</v>
+      </c>
+      <c r="B21" s="11">
+        <v>3</v>
+      </c>
+      <c r="C21" s="12">
+        <v>23212</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>41952</v>
+      </c>
+      <c r="B22" s="11">
+        <v>1</v>
+      </c>
+      <c r="C22" s="12">
+        <v>43476</v>
+      </c>
+      <c r="D22" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>41965</v>
+      </c>
+      <c r="B23" s="11">
+        <v>0</v>
+      </c>
+      <c r="C23" s="12">
+        <v>31825</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>41972</v>
+      </c>
+      <c r="B24" s="11">
+        <v>0</v>
+      </c>
+      <c r="C24" s="12">
+        <v>45232</v>
+      </c>
+      <c r="D24" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>41976</v>
+      </c>
+      <c r="B25" s="11">
+        <v>1</v>
+      </c>
+      <c r="C25" s="12">
+        <v>41152</v>
+      </c>
+      <c r="D25" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>41979</v>
+      </c>
+      <c r="B26" s="11">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12">
+        <v>44716</v>
+      </c>
+      <c r="D26" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>41986</v>
+      </c>
+      <c r="B27" s="11">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12">
+        <v>41694</v>
+      </c>
+      <c r="D27" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>41994</v>
+      </c>
+      <c r="B28" s="11">
+        <v>1</v>
+      </c>
+      <c r="C28" s="12">
+        <v>52315</v>
+      </c>
+      <c r="D28" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>41999</v>
+      </c>
+      <c r="B29" s="11">
+        <v>1</v>
+      </c>
+      <c r="C29" s="12">
+        <v>44817</v>
+      </c>
+      <c r="D29" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>42001</v>
+      </c>
+      <c r="B30" s="11">
+        <v>0</v>
+      </c>
+      <c r="C30" s="12">
+        <v>35436</v>
+      </c>
+      <c r="D30" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>42005</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2</v>
+      </c>
+      <c r="C31" s="12">
+        <v>45367</v>
+      </c>
+      <c r="D31" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>42008</v>
+      </c>
+      <c r="B32" s="11">
+        <v>1</v>
+      </c>
+      <c r="C32" s="12">
+        <v>30302</v>
+      </c>
+      <c r="D32" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>42014</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0</v>
+      </c>
+      <c r="C33" s="12">
+        <v>45369</v>
+      </c>
+      <c r="D33" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>42021</v>
+      </c>
+      <c r="B34" s="11">
+        <v>1</v>
+      </c>
+      <c r="C34" s="12">
+        <v>35973</v>
+      </c>
+      <c r="D34" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>42028</v>
+      </c>
+      <c r="B35" s="11">
+        <v>0</v>
+      </c>
+      <c r="C35" s="12">
+        <v>22961</v>
+      </c>
+      <c r="D35" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="11"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="11"/>
+    </row>
+    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="10"/>
+      <c r="D43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="11"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="11"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11"/>
+    </row>
+    <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A51" s="15"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="10"/>
+      <c r="B53" s="11"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="10"/>
+      <c r="B54" s="11"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="11"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="10"/>
+      <c r="B55" s="11"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="11"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="10"/>
+      <c r="B56" s="11"/>
+      <c r="C56" s="10"/>
+      <c r="D56" s="11"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="10"/>
+      <c r="B57" s="11"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="11"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="10"/>
+      <c r="B58" s="11"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="11"/>
+    </row>
+    <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="10"/>
+      <c r="B62" s="11"/>
+      <c r="C62" s="10"/>
+      <c r="D62" s="11"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="10"/>
+      <c r="B63" s="11"/>
+      <c r="C63" s="10"/>
+      <c r="D63" s="11"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="11"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="10"/>
+      <c r="B65" s="11"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="11"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="10"/>
+      <c r="B66" s="11"/>
+      <c r="C66" s="10"/>
+      <c r="D66" s="11"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="10"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="11"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="10"/>
+      <c r="B68" s="11"/>
+      <c r="C68" s="10"/>
+      <c r="D68" s="11"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="10"/>
+      <c r="B69" s="11"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="11"/>
+    </row>
+    <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+      <c r="A71" s="15"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="11"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="11"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="10"/>
+      <c r="D74" s="11"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="11"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="11"/>
+      <c r="C76" s="10"/>
+      <c r="D76" s="11"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="11"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="11"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="11"/>
+      <c r="C78" s="10"/>
+      <c r="D78" s="11"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="10"/>
+      <c r="B79" s="11"/>
+      <c r="C79" s="10"/>
+      <c r="D79" s="11"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="11"/>
+      <c r="C80" s="10"/>
+      <c r="D80" s="11"/>
+    </row>
+    <row r="82" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A82" s="16"/>
+    </row>
+    <row r="84" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="17"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="18"/>
+    </row>
+    <row r="89" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="17"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="19"/>
+      <c r="B91" s="20"/>
+      <c r="D91" s="20"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="B92" s="11"/>
+      <c r="D92" s="11"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="10"/>
+      <c r="B93" s="11"/>
+      <c r="D93" s="11"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="11"/>
+      <c r="D94" s="11"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="10"/>
+      <c r="B95" s="11"/>
+      <c r="D95" s="11"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="10"/>
+      <c r="B96" s="11"/>
+      <c r="D96" s="11"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="10"/>
+      <c r="B97" s="11"/>
+      <c r="D97" s="11"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="10"/>
+      <c r="B98" s="11"/>
+      <c r="D98" s="11"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="B99" s="11"/>
+      <c r="D99" s="11"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add another column of sample data
</commit_message>
<xml_diff>
--- a/ExcelImport/ExampleSage50Export.xlsx
+++ b/ExcelImport/ExampleSage50Export.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19768" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19769" uniqueCount="681">
   <si>
     <t>No</t>
   </si>
@@ -2066,6 +2066,9 @@
   <si>
     <t>Widgets sold</t>
   </si>
+  <si>
+    <t>Overtime</t>
+  </si>
 </sst>
 </file>
 
@@ -79117,10 +79120,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79132,7 +79135,7 @@
     <col min="5" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
@@ -79145,8 +79148,11 @@
       <c r="D1" s="21" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="21" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>41839</v>
       </c>
@@ -79159,8 +79165,11 @@
       <c r="D2" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>41842</v>
       </c>
@@ -79173,8 +79182,11 @@
       <c r="D3" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>41843</v>
       </c>
@@ -79187,8 +79199,11 @@
       <c r="D4" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>41849</v>
       </c>
@@ -79201,8 +79216,11 @@
       <c r="D5" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>41850</v>
       </c>
@@ -79215,8 +79233,11 @@
       <c r="D6" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>41853</v>
       </c>
@@ -79229,8 +79250,11 @@
       <c r="D7" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>41858</v>
       </c>
@@ -79243,8 +79267,11 @@
       <c r="D8" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>41860</v>
       </c>
@@ -79257,8 +79284,11 @@
       <c r="D9" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>41867</v>
       </c>
@@ -79271,8 +79301,11 @@
       <c r="D10" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>41875</v>
       </c>
@@ -79285,8 +79318,11 @@
       <c r="D11" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>41878</v>
       </c>
@@ -79299,8 +79335,11 @@
       <c r="D12" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>41881</v>
       </c>
@@ -79313,8 +79352,11 @@
       <c r="D13" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>41895</v>
       </c>
@@ -79327,8 +79369,11 @@
       <c r="D14" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>41902</v>
       </c>
@@ -79341,8 +79386,11 @@
       <c r="D15" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>41905</v>
       </c>
@@ -79355,8 +79403,11 @@
       <c r="D16" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
         <v>41909</v>
       </c>
@@ -79369,8 +79420,11 @@
       <c r="D17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>41916</v>
       </c>
@@ -79383,8 +79437,11 @@
       <c r="D18" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>41930</v>
       </c>
@@ -79397,8 +79454,11 @@
       <c r="D19" s="11">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
         <v>41937</v>
       </c>
@@ -79411,8 +79471,11 @@
       <c r="D20" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>41946</v>
       </c>
@@ -79425,8 +79488,11 @@
       <c r="D21" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="9">
         <v>41952</v>
       </c>
@@ -79439,8 +79505,11 @@
       <c r="D22" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>41965</v>
       </c>
@@ -79453,8 +79522,11 @@
       <c r="D23" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>41972</v>
       </c>
@@ -79467,8 +79539,11 @@
       <c r="D24" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>41976</v>
       </c>
@@ -79481,8 +79556,11 @@
       <c r="D25" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="9">
         <v>41979</v>
       </c>
@@ -79495,8 +79573,11 @@
       <c r="D26" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>41986</v>
       </c>
@@ -79509,8 +79590,11 @@
       <c r="D27" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9">
         <v>41994</v>
       </c>
@@ -79523,8 +79607,11 @@
       <c r="D28" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>41999</v>
       </c>
@@ -79537,8 +79624,11 @@
       <c r="D29" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>42001</v>
       </c>
@@ -79551,8 +79641,11 @@
       <c r="D30" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>42005</v>
       </c>
@@ -79565,8 +79658,11 @@
       <c r="D31" s="11">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>42008</v>
       </c>
@@ -79579,8 +79675,11 @@
       <c r="D32" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="9">
         <v>42014</v>
       </c>
@@ -79593,8 +79692,11 @@
       <c r="D33" s="11">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="9">
         <v>42021</v>
       </c>
@@ -79607,8 +79709,11 @@
       <c r="D34" s="11">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>42028</v>
       </c>
@@ -79621,65 +79726,68 @@
       <c r="D35" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="10"/>
       <c r="D36" s="11"/>
     </row>
-    <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="15"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="10"/>
       <c r="D40" s="11"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="10"/>
       <c r="D41" s="11"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="10"/>
       <c r="D42" s="11"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="10"/>
       <c r="D43" s="11"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="10"/>
       <c r="D44" s="11"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="10"/>
       <c r="B45" s="11"/>
       <c r="C45" s="10"/>
       <c r="D45" s="11"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="10"/>
       <c r="B46" s="11"/>
       <c r="C46" s="10"/>
       <c r="D46" s="11"/>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="10"/>
       <c r="D47" s="11"/>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
       <c r="B48" s="11"/>
       <c r="C48" s="10"/>

</xml_diff>